<commit_message>
up 15/11, modify lupusregina
</commit_message>
<xml_diff>
--- a/data/players_priorities.xlsx
+++ b/data/players_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Divide-BiS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BE5437-3281-44F7-9CD2-075845D89A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129ADCC1-C2C2-4B46-B5CF-39D5DA9BCFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="206">
   <si>
     <t>player</t>
   </si>
@@ -121,12 +121,15 @@
     <t>Reputation</t>
   </si>
   <si>
+    <t>Lupusreginä</t>
+  </si>
+  <si>
+    <t>Ashen Band of Endless Destruction</t>
+  </si>
+  <si>
     <t>Pamage</t>
   </si>
   <si>
-    <t>Ashen Band of Endless Destruction</t>
-  </si>
-  <si>
     <t>Darnä</t>
   </si>
   <si>
@@ -139,33 +142,30 @@
     <t>Euphemià</t>
   </si>
   <si>
-    <t>Lupusreginä</t>
-  </si>
-  <si>
     <t>Ashen Band of Endless Might</t>
   </si>
   <si>
+    <t>Dimoncello</t>
+  </si>
+  <si>
+    <t>Ashen Band of Endless Vengeance</t>
+  </si>
+  <si>
+    <t>Drikato</t>
+  </si>
+  <si>
     <t>Aurallia</t>
   </si>
   <si>
-    <t>Ashen Band of Endless Vengeance</t>
-  </si>
-  <si>
     <t>Royalhaze</t>
   </si>
   <si>
-    <t>Dimoncello</t>
-  </si>
-  <si>
-    <t>Drikato</t>
+    <t>Ashen Band of Endless Wisdom</t>
   </si>
   <si>
     <t>Zàpp</t>
   </si>
   <si>
-    <t>Ashen Band of Endless Wisdom</t>
-  </si>
-  <si>
     <t>Seina</t>
   </si>
   <si>
@@ -377,9 +377,6 @@
   </si>
   <si>
     <t>Icecrown Glacial Wall</t>
-  </si>
-  <si>
-    <t>Icecrown Spire Sandals</t>
   </si>
   <si>
     <t>Idol of the Black Willow</t>
@@ -1005,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A425" workbookViewId="0">
-      <selection activeCell="E438" sqref="E438"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="E284" sqref="E284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,6 +1212,9 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1358,7 +1358,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>50402</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B26">
         <v>50402</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>50402</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>50402</v>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>50402</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>50402</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B33">
         <v>50402</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B34">
         <v>50402</v>
@@ -1498,13 +1498,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B35">
         <v>50400</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
         <v>32</v>
@@ -1512,13 +1512,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B36">
         <v>50400</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
         <v>32</v>
@@ -1526,13 +1526,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37">
         <v>50400</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
@@ -1540,13 +1540,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B38">
         <v>50400</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" t="s">
         <v>32</v>
@@ -1554,13 +1554,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B39">
         <v>50400</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
         <v>32</v>
@@ -1568,13 +1568,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B40">
         <v>50400</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>50707</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B47">
         <v>50604</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B52">
         <v>50458</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B53">
         <v>50458</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B56">
         <v>50724</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57">
         <v>50724</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B58">
         <v>50724</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B59">
         <v>50724</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B60">
         <v>50724</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B61">
         <v>50724</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62">
         <v>50724</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B63">
         <v>50724</v>
@@ -1904,10 +1904,13 @@
       <c r="D63" t="s">
         <v>62</v>
       </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B64">
         <v>50724</v>
@@ -1917,9 +1920,6 @@
       </c>
       <c r="D64" t="s">
         <v>63</v>
-      </c>
-      <c r="E64" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -2011,7 +2011,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B71">
         <v>50687</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B73">
         <v>50732</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B74">
         <v>50732</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B75">
         <v>50732</v>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B85">
         <v>50630</v>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B88">
         <v>50616</v>
@@ -2262,6 +2262,9 @@
       </c>
       <c r="D88" t="s">
         <v>7</v>
+      </c>
+      <c r="E88" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2280,7 +2283,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B90">
         <v>50616</v>
@@ -2382,7 +2385,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>21</v>
       </c>
@@ -2396,7 +2399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>21</v>
       </c>
@@ -2410,7 +2413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>21</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>21</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>26</v>
       </c>
@@ -2452,7 +2455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>26</v>
       </c>
@@ -2466,7 +2469,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>26</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -2494,7 +2497,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>51</v>
       </c>
@@ -2507,8 +2510,11 @@
       <c r="D105" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E105" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>51</v>
       </c>
@@ -2522,7 +2528,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>30</v>
       </c>
@@ -2536,7 +2542,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>30</v>
       </c>
@@ -2550,7 +2556,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>30</v>
       </c>
@@ -2564,7 +2570,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -2578,9 +2584,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B111">
         <v>52030</v>
@@ -2592,9 +2598,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B112">
         <v>52030</v>
@@ -2608,7 +2614,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B113">
         <v>52030</v>
@@ -2622,7 +2628,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B114">
         <v>52030</v>
@@ -2636,7 +2642,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B115">
         <v>52030</v>
@@ -2650,7 +2656,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B116">
         <v>52030</v>
@@ -2664,7 +2670,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B117">
         <v>52030</v>
@@ -2678,7 +2684,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B118">
         <v>52030</v>
@@ -2692,7 +2698,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B119">
         <v>52030</v>
@@ -2706,7 +2712,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B120">
         <v>52030</v>
@@ -2720,7 +2726,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B121">
         <v>52030</v>
@@ -2734,7 +2740,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B122">
         <v>52030</v>
@@ -2748,7 +2754,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B123">
         <v>50684</v>
@@ -2762,7 +2768,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B124">
         <v>50684</v>
@@ -2776,7 +2782,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B125">
         <v>50684</v>
@@ -2790,7 +2796,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B126">
         <v>50684</v>
@@ -2832,7 +2838,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B129">
         <v>50613</v>
@@ -2849,7 +2855,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B130">
         <v>50613</v>
@@ -2863,7 +2869,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B131">
         <v>50613</v>
@@ -2877,7 +2883,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B132">
         <v>50613</v>
@@ -2891,7 +2897,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B133">
         <v>50613</v>
@@ -2905,7 +2911,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B134">
         <v>50613</v>
@@ -2919,7 +2925,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B135">
         <v>50613</v>
@@ -2933,7 +2939,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B136">
         <v>50613</v>
@@ -2947,7 +2953,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B137">
         <v>50613</v>
@@ -2961,7 +2967,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B138">
         <v>50721</v>
@@ -3031,7 +3037,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B143">
         <v>50686</v>
@@ -3076,7 +3082,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B146">
         <v>47131</v>
@@ -3093,7 +3099,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B147">
         <v>47131</v>
@@ -3124,7 +3130,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B149">
         <v>47131</v>
@@ -3211,7 +3217,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B155">
         <v>50363</v>
@@ -3225,7 +3231,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B156">
         <v>50363</v>
@@ -3239,7 +3245,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B157">
         <v>50363</v>
@@ -3253,7 +3259,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B158">
         <v>50363</v>
@@ -3368,7 +3374,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B166">
         <v>50348</v>
@@ -3385,7 +3391,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B167">
         <v>50348</v>
@@ -3402,7 +3408,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B168">
         <v>50348</v>
@@ -3416,7 +3422,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B169">
         <v>50348</v>
@@ -3430,7 +3436,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B170">
         <v>50348</v>
@@ -3444,7 +3450,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B171">
         <v>50348</v>
@@ -3486,7 +3492,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B174">
         <v>50733</v>
@@ -3500,7 +3506,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B175">
         <v>50733</v>
@@ -3514,7 +3520,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B176">
         <v>50733</v>
@@ -3528,7 +3534,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B177">
         <v>50733</v>
@@ -3570,7 +3576,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B180">
         <v>50650</v>
@@ -3626,7 +3632,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B184">
         <v>50628</v>
@@ -3640,7 +3646,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B185">
         <v>50628</v>
@@ -3654,7 +3660,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B186">
         <v>50628</v>
@@ -3668,7 +3674,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B187">
         <v>50628</v>
@@ -3682,7 +3688,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B188">
         <v>50628</v>
@@ -3696,7 +3702,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B189">
         <v>50628</v>
@@ -3707,10 +3713,13 @@
       <c r="D189" t="s">
         <v>61</v>
       </c>
+      <c r="E189" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B190">
         <v>50628</v>
@@ -3721,13 +3730,10 @@
       <c r="D190" t="s">
         <v>62</v>
       </c>
-      <c r="E190" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B191">
         <v>50628</v>
@@ -3738,10 +3744,13 @@
       <c r="D191" t="s">
         <v>63</v>
       </c>
+      <c r="E191" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B192">
         <v>50628</v>
@@ -3751,9 +3760,6 @@
       </c>
       <c r="D192" t="s">
         <v>77</v>
-      </c>
-      <c r="E192" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
@@ -3772,7 +3778,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B194">
         <v>50607</v>
@@ -3786,7 +3792,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B195">
         <v>50607</v>
@@ -3800,7 +3806,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B196">
         <v>50607</v>
@@ -3831,7 +3837,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B198">
         <v>50607</v>
@@ -3870,6 +3876,9 @@
       <c r="D200" t="s">
         <v>7</v>
       </c>
+      <c r="E200" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
@@ -3887,7 +3896,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B202">
         <v>50618</v>
@@ -3904,7 +3913,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B203">
         <v>50618</v>
@@ -3918,7 +3927,7 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B204">
         <v>50618</v>
@@ -4148,7 +4157,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B220">
         <v>50736</v>
@@ -4176,7 +4185,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B222">
         <v>50698</v>
@@ -4221,27 +4230,27 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B225">
-        <v>51899</v>
+        <v>50454</v>
       </c>
       <c r="C225" t="s">
         <v>119</v>
       </c>
       <c r="D225" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B226">
         <v>50454</v>
       </c>
       <c r="C226" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D226" t="s">
         <v>55</v>
@@ -4249,10 +4258,10 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B227">
-        <v>50454</v>
+        <v>50456</v>
       </c>
       <c r="C227" t="s">
         <v>120</v>
@@ -4263,10 +4272,10 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B228">
-        <v>50456</v>
+        <v>50457</v>
       </c>
       <c r="C228" t="s">
         <v>121</v>
@@ -4277,52 +4286,52 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B229">
-        <v>50457</v>
+        <v>50656</v>
       </c>
       <c r="C229" t="s">
         <v>122</v>
       </c>
       <c r="D229" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B230">
         <v>50656</v>
       </c>
       <c r="C230" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D230" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B231">
-        <v>50656</v>
+        <v>50642</v>
       </c>
       <c r="C231" t="s">
         <v>123</v>
       </c>
       <c r="D231" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B232">
-        <v>50642</v>
+        <v>51882</v>
       </c>
       <c r="C232" t="s">
         <v>124</v>
@@ -4333,10 +4342,10 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B233">
-        <v>51882</v>
+        <v>50728</v>
       </c>
       <c r="C233" t="s">
         <v>125</v>
@@ -4347,10 +4356,10 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B234">
-        <v>50728</v>
+        <v>50708</v>
       </c>
       <c r="C234" t="s">
         <v>126</v>
@@ -4361,10 +4370,10 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B235">
-        <v>50708</v>
+        <v>50645</v>
       </c>
       <c r="C235" t="s">
         <v>127</v>
@@ -4375,111 +4384,111 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B236">
         <v>50645</v>
       </c>
       <c r="C236" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D236" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B237">
         <v>50645</v>
       </c>
       <c r="C237" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D237" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B238">
-        <v>50645</v>
+        <v>49891</v>
       </c>
       <c r="C238" t="s">
         <v>128</v>
       </c>
       <c r="D238" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="E238" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B239">
-        <v>49891</v>
+        <v>47664</v>
       </c>
       <c r="C239" t="s">
         <v>129</v>
       </c>
       <c r="D239" t="s">
-        <v>58</v>
-      </c>
-      <c r="E239" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B240">
-        <v>47664</v>
+        <v>40705</v>
       </c>
       <c r="C240" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D240" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B241">
         <v>40705</v>
       </c>
       <c r="C241" t="s">
+        <v>131</v>
+      </c>
+      <c r="D241" t="s">
         <v>132</v>
-      </c>
-      <c r="D241" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B242">
-        <v>40705</v>
+        <v>50455</v>
       </c>
       <c r="C242" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D242" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B243">
-        <v>50455</v>
+        <v>50461</v>
       </c>
       <c r="C243" t="s">
         <v>134</v>
@@ -4490,55 +4499,55 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="B244">
-        <v>50461</v>
+        <v>50702</v>
       </c>
       <c r="C244" t="s">
         <v>135</v>
       </c>
       <c r="D244" t="s">
-        <v>55</v>
+        <v>7</v>
+      </c>
+      <c r="E244" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B245">
         <v>50702</v>
       </c>
       <c r="C245" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D245" t="s">
-        <v>7</v>
-      </c>
-      <c r="E245" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B246">
-        <v>50702</v>
+        <v>50621</v>
       </c>
       <c r="C246" t="s">
         <v>136</v>
       </c>
       <c r="D246" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B247">
-        <v>50621</v>
+        <v>50636</v>
       </c>
       <c r="C247" t="s">
         <v>137</v>
@@ -4549,58 +4558,61 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B248">
         <v>50636</v>
       </c>
       <c r="C248" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D248" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B249">
         <v>50636</v>
       </c>
       <c r="C249" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D249" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B250">
-        <v>50636</v>
+        <v>46051</v>
       </c>
       <c r="C250" t="s">
         <v>138</v>
       </c>
       <c r="D250" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="E250" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B251">
         <v>46051</v>
       </c>
       <c r="C251" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D251" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E251" t="s">
         <v>15</v>
@@ -4608,55 +4620,52 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B252">
-        <v>46051</v>
+        <v>50693</v>
       </c>
       <c r="C252" t="s">
         <v>139</v>
       </c>
       <c r="D252" t="s">
-        <v>9</v>
-      </c>
-      <c r="E252" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B253">
         <v>50693</v>
       </c>
       <c r="C253" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D253" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B254">
-        <v>50693</v>
+        <v>50738</v>
       </c>
       <c r="C254" t="s">
         <v>140</v>
       </c>
       <c r="D254" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B255">
-        <v>50738</v>
+        <v>50688</v>
       </c>
       <c r="C255" t="s">
         <v>141</v>
@@ -4667,97 +4676,100 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B256">
         <v>50688</v>
       </c>
       <c r="C256" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D256" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E256" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B257">
         <v>50688</v>
       </c>
       <c r="C257" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D257" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B258">
         <v>50688</v>
       </c>
       <c r="C258" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D258" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="E258" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B259">
-        <v>50688</v>
+        <v>50631</v>
       </c>
       <c r="C259" t="s">
         <v>142</v>
       </c>
       <c r="D259" t="s">
-        <v>18</v>
-      </c>
-      <c r="E259" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B260">
         <v>50631</v>
       </c>
       <c r="C260" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D260" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B261">
-        <v>50631</v>
+        <v>50627</v>
       </c>
       <c r="C261" t="s">
         <v>143</v>
       </c>
       <c r="D261" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B262">
-        <v>50627</v>
+        <v>50735</v>
       </c>
       <c r="C262" t="s">
         <v>144</v>
@@ -4768,307 +4780,310 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B263">
         <v>50735</v>
       </c>
       <c r="C263" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D263" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B264">
         <v>50735</v>
       </c>
       <c r="C264" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D264" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B265">
         <v>50735</v>
       </c>
       <c r="C265" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D265" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B266">
-        <v>50735</v>
+        <v>50365</v>
       </c>
       <c r="C266" t="s">
         <v>145</v>
       </c>
       <c r="D266" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B267">
         <v>50365</v>
       </c>
       <c r="C267" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D267" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B268">
         <v>50365</v>
       </c>
       <c r="C268" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D268" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B269">
         <v>50365</v>
       </c>
       <c r="C269" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D269" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B270">
         <v>50365</v>
       </c>
       <c r="C270" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D270" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B271">
         <v>50365</v>
       </c>
       <c r="C271" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D271" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B272">
-        <v>50365</v>
+        <v>50699</v>
       </c>
       <c r="C272" t="s">
         <v>146</v>
       </c>
       <c r="D272" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B273">
         <v>50699</v>
       </c>
       <c r="C273" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D273" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B274">
         <v>50699</v>
       </c>
       <c r="C274" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D274" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B275">
         <v>50699</v>
       </c>
       <c r="C275" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D275" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B276">
         <v>50699</v>
       </c>
       <c r="C276" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D276" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B277">
         <v>50699</v>
       </c>
       <c r="C277" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D277" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B278">
         <v>50699</v>
       </c>
       <c r="C278" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D278" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B279">
         <v>50699</v>
       </c>
       <c r="C279" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D279" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B280">
         <v>50699</v>
       </c>
       <c r="C280" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D280" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B281">
         <v>50699</v>
       </c>
       <c r="C281" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D281" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B282">
         <v>50699</v>
       </c>
       <c r="C282" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D282" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B283">
         <v>50699</v>
       </c>
       <c r="C283" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D283" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="E283" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B284">
         <v>50694</v>
       </c>
       <c r="C284" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D284" t="s">
         <v>7</v>
@@ -5076,13 +5091,13 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B285">
         <v>50694</v>
       </c>
       <c r="C285" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D285" t="s">
         <v>9</v>
@@ -5090,13 +5105,13 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B286">
         <v>50694</v>
       </c>
       <c r="C286" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D286" t="s">
         <v>11</v>
@@ -5110,7 +5125,7 @@
         <v>50659</v>
       </c>
       <c r="C287" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D287" t="s">
         <v>7</v>
@@ -5127,7 +5142,7 @@
         <v>50659</v>
       </c>
       <c r="C288" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D288" t="s">
         <v>9</v>
@@ -5144,7 +5159,7 @@
         <v>50659</v>
       </c>
       <c r="C289" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D289" t="s">
         <v>11</v>
@@ -5158,7 +5173,7 @@
         <v>51890</v>
       </c>
       <c r="C290" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D290" t="s">
         <v>7</v>
@@ -5172,7 +5187,7 @@
         <v>50705</v>
       </c>
       <c r="C291" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D291" t="s">
         <v>7</v>
@@ -5186,7 +5201,7 @@
         <v>50705</v>
       </c>
       <c r="C292" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D292" t="s">
         <v>9</v>
@@ -5200,7 +5215,7 @@
         <v>52029</v>
       </c>
       <c r="C293" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D293" t="s">
         <v>7</v>
@@ -5217,7 +5232,7 @@
         <v>52029</v>
       </c>
       <c r="C294" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D294" t="s">
         <v>9</v>
@@ -5231,7 +5246,7 @@
         <v>52029</v>
       </c>
       <c r="C295" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D295" t="s">
         <v>11</v>
@@ -5245,7 +5260,7 @@
         <v>52029</v>
       </c>
       <c r="C296" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D296" t="s">
         <v>18</v>
@@ -5259,7 +5274,7 @@
         <v>52029</v>
       </c>
       <c r="C297" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D297" t="s">
         <v>20</v>
@@ -5273,7 +5288,7 @@
         <v>52029</v>
       </c>
       <c r="C298" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D298" t="s">
         <v>60</v>
@@ -5287,7 +5302,7 @@
         <v>52029</v>
       </c>
       <c r="C299" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D299" t="s">
         <v>61</v>
@@ -5301,7 +5316,7 @@
         <v>52029</v>
       </c>
       <c r="C300" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D300" t="s">
         <v>62</v>
@@ -5309,13 +5324,13 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B301">
         <v>52029</v>
       </c>
       <c r="C301" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D301" t="s">
         <v>63</v>
@@ -5323,13 +5338,13 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B302">
         <v>52029</v>
       </c>
       <c r="C302" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D302" t="s">
         <v>77</v>
@@ -5337,13 +5352,13 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B303">
         <v>52029</v>
       </c>
       <c r="C303" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D303" t="s">
         <v>78</v>
@@ -5351,13 +5366,13 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B304">
         <v>52029</v>
       </c>
       <c r="C304" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D304" t="s">
         <v>79</v>
@@ -5365,13 +5380,13 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B305">
         <v>52029</v>
       </c>
       <c r="C305" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D305" t="s">
         <v>80</v>
@@ -5379,13 +5394,13 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B306">
         <v>52029</v>
       </c>
       <c r="C306" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D306" t="s">
         <v>81</v>
@@ -5393,13 +5408,13 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B307">
         <v>52029</v>
       </c>
       <c r="C307" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D307" t="s">
         <v>82</v>
@@ -5407,13 +5422,13 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B308">
         <v>52029</v>
       </c>
       <c r="C308" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D308" t="s">
         <v>83</v>
@@ -5427,7 +5442,7 @@
         <v>52029</v>
       </c>
       <c r="C309" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D309" t="s">
         <v>84</v>
@@ -5441,7 +5456,7 @@
         <v>52029</v>
       </c>
       <c r="C310" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D310" t="s">
         <v>85</v>
@@ -5455,7 +5470,7 @@
         <v>52029</v>
       </c>
       <c r="C311" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D311" t="s">
         <v>86</v>
@@ -5469,7 +5484,7 @@
         <v>52029</v>
       </c>
       <c r="C312" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D312" t="s">
         <v>87</v>
@@ -5477,13 +5492,13 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B313">
         <v>52029</v>
       </c>
       <c r="C313" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D313" t="s">
         <v>88</v>
@@ -5491,13 +5506,13 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B314">
         <v>52029</v>
       </c>
       <c r="C314" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D314" t="s">
         <v>89</v>
@@ -5505,13 +5520,13 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B315">
         <v>52029</v>
       </c>
       <c r="C315" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D315" t="s">
         <v>90</v>
@@ -5519,13 +5534,13 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B316">
         <v>52029</v>
       </c>
       <c r="C316" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D316" t="s">
         <v>91</v>
@@ -5533,13 +5548,13 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B317">
         <v>52029</v>
       </c>
       <c r="C317" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D317" t="s">
         <v>92</v>
@@ -5547,13 +5562,13 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B318">
         <v>52029</v>
       </c>
       <c r="C318" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D318" t="s">
         <v>93</v>
@@ -5561,30 +5576,30 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B319">
         <v>52029</v>
       </c>
       <c r="C319" t="s">
+        <v>151</v>
+      </c>
+      <c r="D319" t="s">
         <v>152</v>
-      </c>
-      <c r="D319" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B320">
         <v>52029</v>
       </c>
       <c r="C320" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D320" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.3">
@@ -5595,10 +5610,10 @@
         <v>52029</v>
       </c>
       <c r="C321" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D321" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.3">
@@ -5609,10 +5624,10 @@
         <v>52029</v>
       </c>
       <c r="C322" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D322" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.3">
@@ -5623,10 +5638,10 @@
         <v>52029</v>
       </c>
       <c r="C323" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D323" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.3">
@@ -5637,10 +5652,10 @@
         <v>52029</v>
       </c>
       <c r="C324" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D324" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.3">
@@ -5651,10 +5666,10 @@
         <v>52029</v>
       </c>
       <c r="C325" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D325" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.3">
@@ -5665,10 +5680,10 @@
         <v>52029</v>
       </c>
       <c r="C326" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D326" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.3">
@@ -5679,10 +5694,10 @@
         <v>52029</v>
       </c>
       <c r="C327" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D327" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.3">
@@ -5693,21 +5708,21 @@
         <v>52029</v>
       </c>
       <c r="C328" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D328" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B329">
         <v>47188</v>
       </c>
       <c r="C329" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D329" t="s">
         <v>7</v>
@@ -5724,7 +5739,7 @@
         <v>50664</v>
       </c>
       <c r="C330" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D330" t="s">
         <v>7</v>
@@ -5732,13 +5747,13 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B331">
         <v>50664</v>
       </c>
       <c r="C331" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D331" t="s">
         <v>9</v>
@@ -5746,13 +5761,13 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B332">
         <v>50664</v>
       </c>
       <c r="C332" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D332" t="s">
         <v>11</v>
@@ -5760,13 +5775,13 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B333">
         <v>50664</v>
       </c>
       <c r="C333" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D333" t="s">
         <v>18</v>
@@ -5774,13 +5789,13 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B334">
         <v>50664</v>
       </c>
       <c r="C334" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D334" t="s">
         <v>20</v>
@@ -5788,13 +5803,13 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B335">
         <v>50664</v>
       </c>
       <c r="C335" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D335" t="s">
         <v>60</v>
@@ -5802,13 +5817,13 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B336">
         <v>50664</v>
       </c>
       <c r="C336" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D336" t="s">
         <v>61</v>
@@ -5816,44 +5831,44 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B337">
         <v>50664</v>
       </c>
       <c r="C337" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D337" t="s">
         <v>62</v>
       </c>
+      <c r="E337" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B338">
         <v>50664</v>
       </c>
       <c r="C338" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D338" t="s">
         <v>63</v>
       </c>
-      <c r="E338" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B339">
         <v>50664</v>
       </c>
       <c r="C339" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D339" t="s">
         <v>77</v>
@@ -5861,13 +5876,13 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B340">
         <v>50629</v>
       </c>
       <c r="C340" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D340" t="s">
         <v>7</v>
@@ -5875,13 +5890,13 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B341">
         <v>50629</v>
       </c>
       <c r="C341" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D341" t="s">
         <v>9</v>
@@ -5892,16 +5907,19 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B342">
         <v>50680</v>
       </c>
       <c r="C342" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D342" t="s">
         <v>7</v>
+      </c>
+      <c r="E342" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.3">
@@ -5912,7 +5930,7 @@
         <v>50680</v>
       </c>
       <c r="C343" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D343" t="s">
         <v>9</v>
@@ -5926,7 +5944,7 @@
         <v>50718</v>
       </c>
       <c r="C344" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D344" t="s">
         <v>7</v>
@@ -5940,7 +5958,7 @@
         <v>50718</v>
       </c>
       <c r="C345" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D345" t="s">
         <v>9</v>
@@ -5954,7 +5972,7 @@
         <v>50734</v>
       </c>
       <c r="C346" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D346" t="s">
         <v>7</v>
@@ -5962,13 +5980,13 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B347">
         <v>50734</v>
       </c>
       <c r="C347" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D347" t="s">
         <v>9</v>
@@ -5976,13 +5994,13 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B348">
         <v>50734</v>
       </c>
       <c r="C348" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D348" t="s">
         <v>11</v>
@@ -5990,13 +6008,13 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B349">
         <v>50734</v>
       </c>
       <c r="C349" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D349" t="s">
         <v>18</v>
@@ -6004,13 +6022,13 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B350">
         <v>50734</v>
       </c>
       <c r="C350" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D350" t="s">
         <v>20</v>
@@ -6018,13 +6036,13 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B351">
         <v>50722</v>
       </c>
       <c r="C351" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D351" t="s">
         <v>7</v>
@@ -6038,7 +6056,7 @@
         <v>50717</v>
       </c>
       <c r="C352" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D352" t="s">
         <v>7</v>
@@ -6052,7 +6070,7 @@
         <v>50717</v>
       </c>
       <c r="C353" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D353" t="s">
         <v>9</v>
@@ -6066,7 +6084,7 @@
         <v>50717</v>
       </c>
       <c r="C354" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D354" t="s">
         <v>11</v>
@@ -6074,13 +6092,13 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B355">
         <v>50655</v>
       </c>
       <c r="C355" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D355" t="s">
         <v>7</v>
@@ -6088,13 +6106,13 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B356">
         <v>50655</v>
       </c>
       <c r="C356" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D356" t="s">
         <v>9</v>
@@ -6102,13 +6120,13 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B357">
         <v>50655</v>
       </c>
       <c r="C357" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D357" t="s">
         <v>11</v>
@@ -6122,7 +6140,7 @@
         <v>50655</v>
       </c>
       <c r="C358" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D358" t="s">
         <v>18</v>
@@ -6136,7 +6154,7 @@
         <v>50624</v>
       </c>
       <c r="C359" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D359" t="s">
         <v>7</v>
@@ -6150,7 +6168,7 @@
         <v>50624</v>
       </c>
       <c r="C360" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D360" t="s">
         <v>9</v>
@@ -6167,7 +6185,7 @@
         <v>50654</v>
       </c>
       <c r="C361" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D361" t="s">
         <v>7</v>
@@ -6184,7 +6202,7 @@
         <v>50678</v>
       </c>
       <c r="C362" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D362" t="s">
         <v>7</v>
@@ -6195,13 +6213,13 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B363">
         <v>50719</v>
       </c>
       <c r="C363" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D363" t="s">
         <v>7</v>
@@ -6209,13 +6227,13 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B364">
         <v>50719</v>
       </c>
       <c r="C364" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D364" t="s">
         <v>9</v>
@@ -6223,13 +6241,13 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B365">
         <v>50719</v>
       </c>
       <c r="C365" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D365" t="s">
         <v>11</v>
@@ -6237,13 +6255,13 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B366">
         <v>50719</v>
       </c>
       <c r="C366" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D366" t="s">
         <v>18</v>
@@ -6251,13 +6269,13 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B367">
         <v>50719</v>
       </c>
       <c r="C367" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D367" t="s">
         <v>20</v>
@@ -6271,13 +6289,13 @@
         <v>49623</v>
       </c>
       <c r="C368" t="s">
+        <v>175</v>
+      </c>
+      <c r="D368" t="s">
         <v>176</v>
       </c>
-      <c r="D368" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>16</v>
       </c>
@@ -6285,27 +6303,27 @@
         <v>50653</v>
       </c>
       <c r="C369" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D369" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B370">
         <v>50653</v>
       </c>
       <c r="C370" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D370" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>8</v>
       </c>
@@ -6313,13 +6331,16 @@
         <v>50653</v>
       </c>
       <c r="C371" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D371" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E371" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>19</v>
       </c>
@@ -6327,13 +6348,13 @@
         <v>50653</v>
       </c>
       <c r="C372" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D372" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>28</v>
       </c>
@@ -6341,13 +6362,13 @@
         <v>50653</v>
       </c>
       <c r="C373" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D373" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>10</v>
       </c>
@@ -6355,13 +6376,13 @@
         <v>47673</v>
       </c>
       <c r="C374" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D374" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>5</v>
       </c>
@@ -6369,13 +6390,13 @@
         <v>50459</v>
       </c>
       <c r="C375" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D375" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>12</v>
       </c>
@@ -6383,13 +6404,13 @@
         <v>50633</v>
       </c>
       <c r="C376" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D376" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>14</v>
       </c>
@@ -6397,13 +6418,13 @@
         <v>50633</v>
       </c>
       <c r="C377" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D377" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>16</v>
       </c>
@@ -6411,69 +6432,69 @@
         <v>50633</v>
       </c>
       <c r="C378" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D378" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B379">
         <v>50633</v>
       </c>
       <c r="C379" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D379" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B380">
         <v>50633</v>
       </c>
       <c r="C380" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D380" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B381">
         <v>50633</v>
       </c>
       <c r="C381" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D381" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B382">
         <v>50633</v>
       </c>
       <c r="C382" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D382" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>17</v>
       </c>
@@ -6481,13 +6502,13 @@
         <v>50633</v>
       </c>
       <c r="C383" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D383" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>51</v>
       </c>
@@ -6495,7 +6516,7 @@
         <v>50364</v>
       </c>
       <c r="C384" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D384" t="s">
         <v>7</v>
@@ -6509,7 +6530,7 @@
         <v>50364</v>
       </c>
       <c r="C385" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D385" t="s">
         <v>9</v>
@@ -6523,7 +6544,7 @@
         <v>50657</v>
       </c>
       <c r="C386" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D386" t="s">
         <v>7</v>
@@ -6540,7 +6561,7 @@
         <v>47059</v>
       </c>
       <c r="C387" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D387" t="s">
         <v>7</v>
@@ -6554,7 +6575,7 @@
         <v>47059</v>
       </c>
       <c r="C388" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D388" t="s">
         <v>9</v>
@@ -6571,7 +6592,7 @@
         <v>47059</v>
       </c>
       <c r="C389" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D389" t="s">
         <v>11</v>
@@ -6588,7 +6609,7 @@
         <v>47059</v>
       </c>
       <c r="C390" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D390" t="s">
         <v>18</v>
@@ -6599,16 +6620,16 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B391">
         <v>37111</v>
       </c>
       <c r="C391" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D391" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.3">
@@ -6619,10 +6640,10 @@
         <v>37111</v>
       </c>
       <c r="C392" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D392" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.3">
@@ -6633,7 +6654,7 @@
         <v>50635</v>
       </c>
       <c r="C393" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D393" t="s">
         <v>7</v>
@@ -6647,7 +6668,7 @@
         <v>50635</v>
       </c>
       <c r="C394" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D394" t="s">
         <v>9</v>
@@ -6661,7 +6682,7 @@
         <v>50635</v>
       </c>
       <c r="C395" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D395" t="s">
         <v>11</v>
@@ -6675,7 +6696,7 @@
         <v>50716</v>
       </c>
       <c r="C396" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D396" t="s">
         <v>7</v>
@@ -6683,13 +6704,13 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B397">
         <v>50651</v>
       </c>
       <c r="C397" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D397" t="s">
         <v>7</v>
@@ -6697,13 +6718,13 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B398">
         <v>50651</v>
       </c>
       <c r="C398" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D398" t="s">
         <v>9</v>
@@ -6711,13 +6732,13 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B399">
         <v>50651</v>
       </c>
       <c r="C399" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D399" t="s">
         <v>11</v>
@@ -6725,13 +6746,13 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B400">
         <v>50706</v>
       </c>
       <c r="C400" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D400" t="s">
         <v>7</v>
@@ -6745,7 +6766,7 @@
         <v>50706</v>
       </c>
       <c r="C401" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D401" t="s">
         <v>9</v>
@@ -6759,7 +6780,7 @@
         <v>50670</v>
       </c>
       <c r="C402" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D402" t="s">
         <v>7</v>
@@ -6773,10 +6794,13 @@
         <v>50670</v>
       </c>
       <c r="C403" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D403" t="s">
         <v>9</v>
+      </c>
+      <c r="E403" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.3">
@@ -6787,7 +6811,7 @@
         <v>50670</v>
       </c>
       <c r="C404" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D404" t="s">
         <v>11</v>
@@ -6795,13 +6819,13 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B405">
         <v>50670</v>
       </c>
       <c r="C405" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D405" t="s">
         <v>18</v>
@@ -6815,7 +6839,7 @@
         <v>50670</v>
       </c>
       <c r="C406" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D406" t="s">
         <v>20</v>
@@ -6829,7 +6853,7 @@
         <v>50670</v>
       </c>
       <c r="C407" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D407" t="s">
         <v>60</v>
@@ -6846,10 +6870,10 @@
         <v>39728</v>
       </c>
       <c r="C408" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D408" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.3">
@@ -6860,7 +6884,7 @@
         <v>50711</v>
       </c>
       <c r="C409" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D409" t="s">
         <v>7</v>
@@ -6874,7 +6898,7 @@
         <v>50703</v>
       </c>
       <c r="C410" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D410" t="s">
         <v>7</v>
@@ -6882,16 +6906,16 @@
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B411">
         <v>46017</v>
       </c>
       <c r="C411" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D411" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E411" t="s">
         <v>15</v>
@@ -6905,10 +6929,10 @@
         <v>46017</v>
       </c>
       <c r="C412" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D412" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E412" t="s">
         <v>15</v>
@@ -6916,30 +6940,33 @@
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B413">
         <v>46017</v>
       </c>
       <c r="C413" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D413" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="E413" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B414">
         <v>46017</v>
       </c>
       <c r="C414" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D414" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E414" t="s">
         <v>15</v>
@@ -6947,19 +6974,16 @@
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="B415">
         <v>46017</v>
       </c>
       <c r="C415" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D415" t="s">
-        <v>177</v>
-      </c>
-      <c r="E415" t="s">
-        <v>15</v>
+        <v>176</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.3">
@@ -6970,7 +6994,7 @@
         <v>50714</v>
       </c>
       <c r="C416" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D416" t="s">
         <v>7</v>
@@ -6984,7 +7008,7 @@
         <v>52028</v>
       </c>
       <c r="C417" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D417" t="s">
         <v>7</v>
@@ -6998,7 +7022,7 @@
         <v>52028</v>
       </c>
       <c r="C418" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D418" t="s">
         <v>9</v>
@@ -7012,7 +7036,7 @@
         <v>52028</v>
       </c>
       <c r="C419" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D419" t="s">
         <v>11</v>
@@ -7026,7 +7050,7 @@
         <v>52028</v>
       </c>
       <c r="C420" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D420" t="s">
         <v>18</v>
@@ -7040,7 +7064,7 @@
         <v>52028</v>
       </c>
       <c r="C421" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D421" t="s">
         <v>20</v>
@@ -7057,7 +7081,7 @@
         <v>52028</v>
       </c>
       <c r="C422" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D422" t="s">
         <v>60</v>
@@ -7071,7 +7095,7 @@
         <v>52028</v>
       </c>
       <c r="C423" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D423" t="s">
         <v>61</v>
@@ -7085,7 +7109,7 @@
         <v>52028</v>
       </c>
       <c r="C424" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D424" t="s">
         <v>62</v>
@@ -7093,13 +7117,13 @@
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B425">
         <v>52028</v>
       </c>
       <c r="C425" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D425" t="s">
         <v>63</v>
@@ -7107,13 +7131,13 @@
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B426">
         <v>52028</v>
       </c>
       <c r="C426" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D426" t="s">
         <v>77</v>
@@ -7121,13 +7145,13 @@
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B427">
         <v>52028</v>
       </c>
       <c r="C427" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D427" t="s">
         <v>78</v>
@@ -7135,13 +7159,13 @@
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B428">
         <v>52028</v>
       </c>
       <c r="C428" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D428" t="s">
         <v>79</v>
@@ -7155,7 +7179,7 @@
         <v>52028</v>
       </c>
       <c r="C429" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D429" t="s">
         <v>80</v>
@@ -7169,7 +7193,7 @@
         <v>52028</v>
       </c>
       <c r="C430" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D430" t="s">
         <v>81</v>
@@ -7183,7 +7207,7 @@
         <v>52028</v>
       </c>
       <c r="C431" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D431" t="s">
         <v>82</v>
@@ -7197,7 +7221,7 @@
         <v>52028</v>
       </c>
       <c r="C432" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D432" t="s">
         <v>83</v>
@@ -7205,13 +7229,13 @@
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B433">
         <v>52028</v>
       </c>
       <c r="C433" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D433" t="s">
         <v>84</v>
@@ -7222,13 +7246,13 @@
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B434">
         <v>52028</v>
       </c>
       <c r="C434" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D434" t="s">
         <v>85</v>
@@ -7236,13 +7260,13 @@
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B435">
         <v>52028</v>
       </c>
       <c r="C435" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D435" t="s">
         <v>86</v>
@@ -7250,13 +7274,13 @@
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B436">
         <v>52028</v>
       </c>
       <c r="C436" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D436" t="s">
         <v>87</v>
@@ -7264,13 +7288,13 @@
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B437">
         <v>52028</v>
       </c>
       <c r="C437" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D437" t="s">
         <v>88</v>
@@ -7281,13 +7305,13 @@
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B438">
         <v>52028</v>
       </c>
       <c r="C438" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D438" t="s">
         <v>89</v>
@@ -7295,13 +7319,13 @@
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B439">
         <v>52028</v>
       </c>
       <c r="C439" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D439" t="s">
         <v>90</v>
@@ -7309,13 +7333,13 @@
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B440">
         <v>52028</v>
       </c>
       <c r="C440" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D440" t="s">
         <v>91</v>
@@ -7323,13 +7347,13 @@
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B441">
         <v>52028</v>
       </c>
       <c r="C441" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D441" t="s">
         <v>92</v>
@@ -7337,13 +7361,13 @@
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B442">
         <v>52028</v>
       </c>
       <c r="C442" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D442" t="s">
         <v>93</v>
@@ -7351,30 +7375,30 @@
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B443">
         <v>52028</v>
       </c>
       <c r="C443" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D443" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B444">
         <v>52028</v>
       </c>
       <c r="C444" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D444" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.3">
@@ -7385,10 +7409,10 @@
         <v>52028</v>
       </c>
       <c r="C445" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D445" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.3">
@@ -7399,66 +7423,66 @@
         <v>52028</v>
       </c>
       <c r="C446" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D446" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B447">
         <v>52028</v>
       </c>
       <c r="C447" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D447" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B448">
         <v>52028</v>
       </c>
       <c r="C448" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D448" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B449">
         <v>52028</v>
       </c>
       <c r="C449" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D449" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B450">
         <v>52028</v>
       </c>
       <c r="C450" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D450" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.3">
@@ -7469,10 +7493,10 @@
         <v>52028</v>
       </c>
       <c r="C451" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D451" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.3">
@@ -7483,10 +7507,10 @@
         <v>52028</v>
       </c>
       <c r="C452" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D452" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.3">
@@ -7497,10 +7521,10 @@
         <v>52028</v>
       </c>
       <c r="C453" t="s">
+        <v>195</v>
+      </c>
+      <c r="D453" t="s">
         <v>196</v>
-      </c>
-      <c r="D453" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.3">
@@ -7511,10 +7535,10 @@
         <v>52028</v>
       </c>
       <c r="C454" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D454" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.3">
@@ -7525,10 +7549,10 @@
         <v>52028</v>
       </c>
       <c r="C455" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D455" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.3">
@@ -7539,10 +7563,10 @@
         <v>52028</v>
       </c>
       <c r="C456" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D456" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.3">
@@ -7553,10 +7577,10 @@
         <v>52028</v>
       </c>
       <c r="C457" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D457" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.3">
@@ -7567,10 +7591,10 @@
         <v>52028</v>
       </c>
       <c r="C458" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D458" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.3">
@@ -7581,7 +7605,7 @@
         <v>47545</v>
       </c>
       <c r="C459" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D459" t="s">
         <v>7</v>
@@ -7595,7 +7619,7 @@
         <v>47545</v>
       </c>
       <c r="C460" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D460" t="s">
         <v>9</v>
@@ -7603,13 +7627,13 @@
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B461">
         <v>47545</v>
       </c>
       <c r="C461" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D461" t="s">
         <v>11</v>
@@ -7617,13 +7641,13 @@
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B462">
         <v>47545</v>
       </c>
       <c r="C462" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D462" t="s">
         <v>18</v>
@@ -7631,13 +7655,13 @@
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B463">
         <v>47545</v>
       </c>
       <c r="C463" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D463" t="s">
         <v>20</v>
@@ -7651,7 +7675,7 @@
         <v>47545</v>
       </c>
       <c r="C464" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D464" t="s">
         <v>60</v>
@@ -7665,7 +7689,7 @@
         <v>51946</v>
       </c>
       <c r="C465" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D465" t="s">
         <v>7</v>
@@ -7679,7 +7703,7 @@
         <v>50343</v>
       </c>
       <c r="C466" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D466" t="s">
         <v>7</v>
@@ -7696,7 +7720,7 @@
         <v>50343</v>
       </c>
       <c r="C467" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D467" t="s">
         <v>9</v>
@@ -7713,7 +7737,7 @@
         <v>50343</v>
       </c>
       <c r="C468" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D468" t="s">
         <v>11</v>
@@ -7727,7 +7751,7 @@
         <v>50343</v>
       </c>
       <c r="C469" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D469" t="s">
         <v>18</v>
@@ -7741,7 +7765,7 @@
         <v>50343</v>
       </c>
       <c r="C470" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D470" t="s">
         <v>20</v>
@@ -7755,7 +7779,7 @@
         <v>50677</v>
       </c>
       <c r="C471" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D471" t="s">
         <v>7</v>
@@ -7772,7 +7796,7 @@
         <v>50677</v>
       </c>
       <c r="C472" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D472" t="s">
         <v>9</v>

</xml_diff>